<commit_message>
updated feedback and deliverables
</commit_message>
<xml_diff>
--- a/Derek LPE Inverter/Derek Feedback.xlsx
+++ b/Derek LPE Inverter/Derek Feedback.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,9 +66,6 @@
     <t>No Version on Review List</t>
   </si>
   <si>
-    <t>Add a version</t>
-  </si>
-  <si>
     <t>It is unclear what Spec refers too</t>
   </si>
   <si>
@@ -259,6 +256,9 @@
   </si>
   <si>
     <t>Spell check!!</t>
+  </si>
+  <si>
+    <t>Consider adding a version even if this is only for internal use</t>
   </si>
 </sst>
 </file>
@@ -339,8 +339,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -416,7 +418,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -438,6 +440,7 @@
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -459,6 +462,7 @@
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -790,8 +794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" zoomScalePageLayoutView="205" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -889,7 +893,7 @@
         <v>14</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>15</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -903,10 +907,10 @@
         <v>13</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -920,10 +924,10 @@
         <v>13</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="32">
@@ -937,10 +941,10 @@
         <v>13</v>
       </c>
       <c r="D10" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="11" t="s">
         <v>17</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -954,10 +958,10 @@
         <v>13</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -971,10 +975,10 @@
         <v>13</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -988,10 +992,10 @@
         <v>13</v>
       </c>
       <c r="D13" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="11" t="s">
         <v>21</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -999,16 +1003,16 @@
         <v>1</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>15</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="48">
@@ -1016,16 +1020,16 @@
         <v>1</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>13</v>
       </c>
       <c r="D15" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="11" t="s">
         <v>26</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1033,16 +1037,16 @@
         <v>1</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="E16" s="11" t="s">
         <v>30</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="32">
@@ -1050,16 +1054,16 @@
         <v>1</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D17" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="11" t="s">
         <v>32</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1067,16 +1071,16 @@
         <v>1</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D18" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="11" t="s">
         <v>34</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1084,16 +1088,16 @@
         <v>1</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1101,16 +1105,16 @@
         <v>1</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="32">
@@ -1118,16 +1122,16 @@
         <v>1</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D21" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E21" s="11" t="s">
         <v>72</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1135,16 +1139,16 @@
         <v>1</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D22" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" s="11" t="s">
         <v>38</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="32">
@@ -1152,16 +1156,16 @@
         <v>1</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D23" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="11" t="s">
         <v>40</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="32">
@@ -1169,16 +1173,16 @@
         <v>1</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D24" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24" s="11" t="s">
         <v>59</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1189,13 +1193,13 @@
         <v>4</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1206,13 +1210,13 @@
         <v>4</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="112">
@@ -1223,13 +1227,13 @@
         <v>4</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="32">
@@ -1240,13 +1244,13 @@
         <v>4</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="32">
@@ -1257,13 +1261,13 @@
         <v>4</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="160">
@@ -1274,13 +1278,13 @@
         <v>4</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1291,13 +1295,13 @@
         <v>4</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D31" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31" s="11" t="s">
         <v>45</v>
-      </c>
-      <c r="E31" s="11" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1308,13 +1312,13 @@
         <v>4</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="80">
@@ -1325,13 +1329,13 @@
         <v>4</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D33" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E33" s="11" t="s">
         <v>65</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="32">
@@ -1342,13 +1346,13 @@
         <v>4</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1359,13 +1363,13 @@
         <v>4</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D35" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E35" s="11" t="s">
         <v>48</v>
-      </c>
-      <c r="E35" s="11" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="32">
@@ -1376,13 +1380,13 @@
         <v>4</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D36" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E36" s="11" t="s">
         <v>50</v>
-      </c>
-      <c r="E36" s="11" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1393,13 +1397,13 @@
         <v>4</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1410,13 +1414,13 @@
         <v>4</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="32">
@@ -1427,13 +1431,13 @@
         <v>4</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>